<commit_message>
feat: add 6.1, add 1/3 solution to 9.1.xlsx
</commit_message>
<xml_diff>
--- a/EGE/reshege-7907903/9_27522.xlsx
+++ b/EGE/reshege-7907903/9_27522.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/reshege-7907903/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B27DCF-A906-494A-8AC5-55D705201D44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист3" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>ЕСЛИ(B2:Y2 &lt; (Z2/2))</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -379,26 +390,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:Y1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -471,8 +482,11 @@
       <c r="Y1" s="1">
         <v>0.95833333333333404</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44287</v>
       </c>
@@ -548,8 +562,15 @@
       <c r="Y2" s="4">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z2" s="4">
+        <f>MAX(Y2,X2,W2,V2,U2,T2,S2,B2:S2)</f>
+        <v>26.4</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44288</v>
       </c>
@@ -625,8 +646,12 @@
       <c r="Y3" s="4">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z3" s="4">
+        <f t="shared" ref="Z3:Z66" si="0">MAX(Y3,X3,W3,V3,U3,T3,S3,B3:S3)</f>
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44289</v>
       </c>
@@ -702,9 +727,13 @@
       <c r="Y4" s="4">
         <v>16.5</v>
       </c>
+      <c r="Z4" s="4">
+        <f t="shared" si="0"/>
+        <v>26.2</v>
+      </c>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44290</v>
       </c>
@@ -780,9 +809,13 @@
       <c r="Y5" s="4">
         <v>15.6</v>
       </c>
+      <c r="Z5" s="4">
+        <f t="shared" si="0"/>
+        <v>26.7</v>
+      </c>
       <c r="AA5" s="4"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44291</v>
       </c>
@@ -858,8 +891,12 @@
       <c r="Y6" s="4">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z6" s="4">
+        <f t="shared" si="0"/>
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44292</v>
       </c>
@@ -935,8 +972,12 @@
       <c r="Y7" s="4">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z7" s="4">
+        <f t="shared" si="0"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44293</v>
       </c>
@@ -1012,8 +1053,12 @@
       <c r="Y8" s="4">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z8" s="4">
+        <f t="shared" si="0"/>
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44294</v>
       </c>
@@ -1089,9 +1134,12 @@
       <c r="Y9" s="4">
         <v>17</v>
       </c>
-      <c r="Z9" s="4"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z9" s="4">
+        <f t="shared" si="0"/>
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44295</v>
       </c>
@@ -1167,8 +1215,12 @@
       <c r="Y10" s="4">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z10" s="4">
+        <f t="shared" si="0"/>
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44296</v>
       </c>
@@ -1244,8 +1296,12 @@
       <c r="Y11" s="4">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z11" s="4">
+        <f t="shared" si="0"/>
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44297</v>
       </c>
@@ -1321,9 +1377,13 @@
       <c r="Y12" s="4">
         <v>15</v>
       </c>
+      <c r="Z12" s="4">
+        <f t="shared" si="0"/>
+        <v>25.9</v>
+      </c>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44298</v>
       </c>
@@ -1399,9 +1459,13 @@
       <c r="Y13" s="4">
         <v>15.8</v>
       </c>
+      <c r="Z13" s="4">
+        <f t="shared" si="0"/>
+        <v>26.9</v>
+      </c>
       <c r="AA13" s="4"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44299</v>
       </c>
@@ -1477,8 +1541,12 @@
       <c r="Y14" s="4">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z14" s="4">
+        <f t="shared" si="0"/>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44300</v>
       </c>
@@ -1554,8 +1622,12 @@
       <c r="Y15" s="4">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z15" s="4">
+        <f t="shared" si="0"/>
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44301</v>
       </c>
@@ -1631,8 +1703,12 @@
       <c r="Y16" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16" s="4">
+        <f t="shared" si="0"/>
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44302</v>
       </c>
@@ -1708,8 +1784,12 @@
       <c r="Y17" s="4">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="4">
+        <f t="shared" si="0"/>
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44303</v>
       </c>
@@ -1785,8 +1865,12 @@
       <c r="Y18" s="4">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="4">
+        <f t="shared" si="0"/>
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44304</v>
       </c>
@@ -1862,8 +1946,12 @@
       <c r="Y19" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="4">
+        <f t="shared" si="0"/>
+        <v>26.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44305</v>
       </c>
@@ -1939,8 +2027,12 @@
       <c r="Y20" s="4">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20" s="4">
+        <f t="shared" si="0"/>
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44306</v>
       </c>
@@ -2016,8 +2108,12 @@
       <c r="Y21" s="4">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" s="4">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44307</v>
       </c>
@@ -2093,8 +2189,12 @@
       <c r="Y22" s="4">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22" s="4">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44308</v>
       </c>
@@ -2170,8 +2270,12 @@
       <c r="Y23" s="4">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" s="4">
+        <f t="shared" si="0"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44311</v>
       </c>
@@ -2247,8 +2351,12 @@
       <c r="Y24" s="4">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24" s="4">
+        <f t="shared" si="0"/>
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44312</v>
       </c>
@@ -2324,8 +2432,12 @@
       <c r="Y25" s="4">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25" s="4">
+        <f t="shared" si="0"/>
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44311</v>
       </c>
@@ -2401,8 +2513,12 @@
       <c r="Y26" s="4">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="4">
+        <f t="shared" si="0"/>
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44312</v>
       </c>
@@ -2478,8 +2594,12 @@
       <c r="Y27" s="4">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z27" s="4">
+        <f t="shared" si="0"/>
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44313</v>
       </c>
@@ -2555,8 +2675,12 @@
       <c r="Y28" s="4">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z28" s="4">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44314</v>
       </c>
@@ -2632,8 +2756,12 @@
       <c r="Y29" s="4">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z29" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44315</v>
       </c>
@@ -2709,8 +2837,12 @@
       <c r="Y30" s="4">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z30" s="4">
+        <f t="shared" si="0"/>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44316</v>
       </c>
@@ -2786,8 +2918,12 @@
       <c r="Y31" s="4">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z31" s="4">
+        <f t="shared" si="0"/>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44317</v>
       </c>
@@ -2863,8 +2999,12 @@
       <c r="Y32" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32" s="4">
+        <f t="shared" si="0"/>
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44318</v>
       </c>
@@ -2940,8 +3080,12 @@
       <c r="Y33" s="4">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="4">
+        <f t="shared" si="0"/>
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44319</v>
       </c>
@@ -3017,8 +3161,12 @@
       <c r="Y34" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44320</v>
       </c>
@@ -3094,8 +3242,12 @@
       <c r="Y35" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="4">
+        <f t="shared" si="0"/>
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44321</v>
       </c>
@@ -3171,8 +3323,12 @@
       <c r="Y36" s="4">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z36" s="4">
+        <f t="shared" si="0"/>
+        <v>30.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44322</v>
       </c>
@@ -3248,8 +3404,12 @@
       <c r="Y37" s="4">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="4">
+        <f t="shared" si="0"/>
+        <v>30.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44323</v>
       </c>
@@ -3325,8 +3485,12 @@
       <c r="Y38" s="4">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38" s="4">
+        <f t="shared" si="0"/>
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44324</v>
       </c>
@@ -3402,8 +3566,12 @@
       <c r="Y39" s="4">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z39" s="4">
+        <f t="shared" si="0"/>
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44325</v>
       </c>
@@ -3479,8 +3647,12 @@
       <c r="Y40" s="4">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40" s="4">
+        <f t="shared" si="0"/>
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44326</v>
       </c>
@@ -3556,8 +3728,12 @@
       <c r="Y41" s="4">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41" s="4">
+        <f t="shared" si="0"/>
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44327</v>
       </c>
@@ -3633,8 +3809,12 @@
       <c r="Y42" s="4">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z42" s="4">
+        <f t="shared" si="0"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44328</v>
       </c>
@@ -3710,8 +3890,12 @@
       <c r="Y43" s="4">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z43" s="4">
+        <f t="shared" si="0"/>
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44329</v>
       </c>
@@ -3787,8 +3971,12 @@
       <c r="Y44" s="4">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z44" s="4">
+        <f t="shared" si="0"/>
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44330</v>
       </c>
@@ -3864,8 +4052,12 @@
       <c r="Y45" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z45" s="4">
+        <f t="shared" si="0"/>
+        <v>30.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44331</v>
       </c>
@@ -3941,8 +4133,12 @@
       <c r="Y46" s="4">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z46" s="4">
+        <f t="shared" si="0"/>
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44332</v>
       </c>
@@ -4018,8 +4214,12 @@
       <c r="Y47" s="4">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z47" s="4">
+        <f t="shared" si="0"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44333</v>
       </c>
@@ -4095,8 +4295,12 @@
       <c r="Y48" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z48" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44334</v>
       </c>
@@ -4172,8 +4376,12 @@
       <c r="Y49" s="4">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z49" s="4">
+        <f t="shared" si="0"/>
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44335</v>
       </c>
@@ -4249,8 +4457,12 @@
       <c r="Y50" s="4">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z50" s="4">
+        <f t="shared" si="0"/>
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44336</v>
       </c>
@@ -4326,8 +4538,12 @@
       <c r="Y51" s="4">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z51" s="4">
+        <f t="shared" si="0"/>
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44337</v>
       </c>
@@ -4403,8 +4619,12 @@
       <c r="Y52" s="4">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z52" s="4">
+        <f t="shared" si="0"/>
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44338</v>
       </c>
@@ -4480,8 +4700,12 @@
       <c r="Y53" s="4">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z53" s="4">
+        <f t="shared" si="0"/>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
@@ -4557,8 +4781,12 @@
       <c r="Y54" s="4">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z54" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
@@ -4634,8 +4862,12 @@
       <c r="Y55" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z55" s="4">
+        <f t="shared" si="0"/>
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44341</v>
       </c>
@@ -4711,8 +4943,12 @@
       <c r="Y56" s="4">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z56" s="4">
+        <f t="shared" si="0"/>
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44342</v>
       </c>
@@ -4788,8 +5024,12 @@
       <c r="Y57" s="4">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z57" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44343</v>
       </c>
@@ -4865,8 +5105,12 @@
       <c r="Y58" s="4">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z58" s="4">
+        <f t="shared" si="0"/>
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44344</v>
       </c>
@@ -4942,8 +5186,12 @@
       <c r="Y59" s="4">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z59" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44345</v>
       </c>
@@ -5019,8 +5267,12 @@
       <c r="Y60" s="4">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z60" s="4">
+        <f t="shared" si="0"/>
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44346</v>
       </c>
@@ -5096,8 +5348,12 @@
       <c r="Y61" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z61" s="4">
+        <f t="shared" si="0"/>
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44347</v>
       </c>
@@ -5173,8 +5429,12 @@
       <c r="Y62" s="4">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z62" s="4">
+        <f t="shared" si="0"/>
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44348</v>
       </c>
@@ -5250,8 +5510,12 @@
       <c r="Y63" s="4">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z63" s="4">
+        <f t="shared" si="0"/>
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44349</v>
       </c>
@@ -5327,8 +5591,12 @@
       <c r="Y64" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z64" s="4">
+        <f t="shared" si="0"/>
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44350</v>
       </c>
@@ -5404,8 +5672,12 @@
       <c r="Y65" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z65" s="4">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44351</v>
       </c>
@@ -5481,8 +5753,12 @@
       <c r="Y66" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z66" s="4">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44352</v>
       </c>
@@ -5558,8 +5834,12 @@
       <c r="Y67" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z67" s="4">
+        <f t="shared" ref="Z67:Z92" si="1">MAX(Y67,X67,W67,V67,U67,T67,S67,B67:S67)</f>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44353</v>
       </c>
@@ -5635,8 +5915,12 @@
       <c r="Y68" s="4">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z68" s="4">
+        <f t="shared" si="1"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44354</v>
       </c>
@@ -5712,8 +5996,12 @@
       <c r="Y69" s="4">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z69" s="4">
+        <f t="shared" si="1"/>
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44355</v>
       </c>
@@ -5789,8 +6077,12 @@
       <c r="Y70" s="4">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z70" s="4">
+        <f t="shared" si="1"/>
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44356</v>
       </c>
@@ -5866,8 +6158,12 @@
       <c r="Y71" s="4">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z71" s="4">
+        <f t="shared" si="1"/>
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44357</v>
       </c>
@@ -5943,8 +6239,12 @@
       <c r="Y72" s="4">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z72" s="4">
+        <f t="shared" si="1"/>
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44358</v>
       </c>
@@ -6020,8 +6320,12 @@
       <c r="Y73" s="4">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z73" s="4">
+        <f t="shared" si="1"/>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44359</v>
       </c>
@@ -6097,8 +6401,12 @@
       <c r="Y74" s="4">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z74" s="4">
+        <f t="shared" si="1"/>
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44360</v>
       </c>
@@ -6174,8 +6482,12 @@
       <c r="Y75" s="4">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z75" s="4">
+        <f t="shared" si="1"/>
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44361</v>
       </c>
@@ -6251,8 +6563,12 @@
       <c r="Y76" s="4">
         <v>28.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z76" s="4">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44362</v>
       </c>
@@ -6328,8 +6644,12 @@
       <c r="Y77" s="4">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z77" s="4">
+        <f t="shared" si="1"/>
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44363</v>
       </c>
@@ -6405,8 +6725,12 @@
       <c r="Y78" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z78" s="4">
+        <f t="shared" si="1"/>
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44364</v>
       </c>
@@ -6482,8 +6806,12 @@
       <c r="Y79" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z79" s="4">
+        <f t="shared" si="1"/>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44365</v>
       </c>
@@ -6559,8 +6887,12 @@
       <c r="Y80" s="4">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z80" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44366</v>
       </c>
@@ -6636,8 +6968,12 @@
       <c r="Y81" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z81" s="4">
+        <f t="shared" si="1"/>
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44367</v>
       </c>
@@ -6713,8 +7049,12 @@
       <c r="Y82" s="4">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z82" s="4">
+        <f t="shared" si="1"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44368</v>
       </c>
@@ -6790,8 +7130,12 @@
       <c r="Y83" s="4">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z83" s="4">
+        <f t="shared" si="1"/>
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44369</v>
       </c>
@@ -6867,8 +7211,12 @@
       <c r="Y84" s="4">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z84" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44372</v>
       </c>
@@ -6944,8 +7292,12 @@
       <c r="Y85" s="4">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z85" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44373</v>
       </c>
@@ -7021,8 +7373,12 @@
       <c r="Y86" s="4">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z86" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44372</v>
       </c>
@@ -7098,8 +7454,12 @@
       <c r="Y87" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z87" s="4">
+        <f t="shared" si="1"/>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44373</v>
       </c>
@@ -7175,8 +7535,12 @@
       <c r="Y88" s="4">
         <v>28.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z88" s="4">
+        <f t="shared" si="1"/>
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44374</v>
       </c>
@@ -7252,8 +7616,12 @@
       <c r="Y89" s="4">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z89" s="4">
+        <f t="shared" si="1"/>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44375</v>
       </c>
@@ -7329,8 +7697,12 @@
       <c r="Y90" s="4">
         <v>27.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z90" s="4">
+        <f t="shared" si="1"/>
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44376</v>
       </c>
@@ -7406,8 +7778,12 @@
       <c r="Y91" s="4">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z91" s="4">
+        <f t="shared" si="1"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44377</v>
       </c>
@@ -7483,14 +7859,18 @@
       <c r="Y92" s="4">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z92" s="4">
+        <f t="shared" si="1"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: OV add solution to 9.1, Excel
</commit_message>
<xml_diff>
--- a/EGE/reshege-7907903/9_27522.xlsx
+++ b/EGE/reshege-7907903/9_27522.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/reshege-7907903/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\ege\EGE\reshege-7907903\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B27DCF-A906-494A-8AC5-55D705201D44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2360A2D3-8B00-43A7-AA04-AC3072AAEC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист3" sheetId="3" r:id="rId1"/>
@@ -144,7 +144,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -196,7 +196,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -401,15 +401,15 @@
   <dimension ref="A1:AA97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -486,7 +486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44287</v>
       </c>
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44288</v>
       </c>
@@ -651,7 +651,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44289</v>
       </c>
@@ -731,9 +731,12 @@
         <f t="shared" si="0"/>
         <v>26.2</v>
       </c>
-      <c r="AA4" s="4"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA4" s="4">
+        <f>COUNTIF(B2:Y92,"&lt;19,5")</f>
+        <v>601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44290</v>
       </c>
@@ -815,7 +818,7 @@
       </c>
       <c r="AA5" s="4"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44291</v>
       </c>
@@ -896,7 +899,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44292</v>
       </c>
@@ -977,7 +980,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44293</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44294</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44295</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44296</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44297</v>
       </c>
@@ -1383,7 +1386,7 @@
       </c>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44298</v>
       </c>
@@ -1465,7 +1468,7 @@
       </c>
       <c r="AA13" s="4"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44299</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44300</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44301</v>
       </c>
@@ -1708,7 +1711,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44302</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44303</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44304</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44305</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>26.3</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44306</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44307</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44308</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44311</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44312</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44311</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44312</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44313</v>
       </c>
@@ -2680,7 +2683,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44314</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44315</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44316</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44317</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44318</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44319</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44320</v>
       </c>
@@ -3247,7 +3250,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44321</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44322</v>
       </c>
@@ -3409,7 +3412,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44323</v>
       </c>
@@ -3490,7 +3493,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44324</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44325</v>
       </c>
@@ -3652,7 +3655,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>44326</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>44327</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>44328</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>44329</v>
       </c>
@@ -3976,7 +3979,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44330</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44331</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>44332</v>
       </c>
@@ -4219,7 +4222,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44333</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>44334</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>44335</v>
       </c>
@@ -4462,7 +4465,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>44336</v>
       </c>
@@ -4543,7 +4546,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>44337</v>
       </c>
@@ -4624,7 +4627,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>44338</v>
       </c>
@@ -4705,7 +4708,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44341</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>44342</v>
       </c>
@@ -4867,7 +4870,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>44341</v>
       </c>
@@ -4948,7 +4951,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44342</v>
       </c>
@@ -5029,7 +5032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>44343</v>
       </c>
@@ -5110,7 +5113,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>44344</v>
       </c>
@@ -5191,7 +5194,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>44345</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>44346</v>
       </c>
@@ -5353,7 +5356,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>44347</v>
       </c>
@@ -5434,7 +5437,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>44348</v>
       </c>
@@ -5515,7 +5518,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>44349</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>44350</v>
       </c>
@@ -5677,7 +5680,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>44351</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>44352</v>
       </c>
@@ -5839,7 +5842,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>44353</v>
       </c>
@@ -5920,7 +5923,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>44354</v>
       </c>
@@ -6001,7 +6004,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>44355</v>
       </c>
@@ -6082,7 +6085,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>44356</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44357</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>44358</v>
       </c>
@@ -6325,7 +6328,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>44359</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>44360</v>
       </c>
@@ -6487,7 +6490,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>44361</v>
       </c>
@@ -6568,7 +6571,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>44362</v>
       </c>
@@ -6649,7 +6652,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>44363</v>
       </c>
@@ -6730,7 +6733,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>44364</v>
       </c>
@@ -6811,7 +6814,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44365</v>
       </c>
@@ -6892,7 +6895,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44366</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>44367</v>
       </c>
@@ -7054,7 +7057,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>44368</v>
       </c>
@@ -7135,7 +7138,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>44369</v>
       </c>
@@ -7216,7 +7219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>44372</v>
       </c>
@@ -7297,7 +7300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>44373</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>44372</v>
       </c>
@@ -7459,7 +7462,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>44373</v>
       </c>
@@ -7540,7 +7543,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>44374</v>
       </c>
@@ -7621,7 +7624,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>44375</v>
       </c>
@@ -7702,7 +7705,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>44376</v>
       </c>
@@ -7783,7 +7786,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>44377</v>
       </c>
@@ -7864,13 +7867,13 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="5"/>
     </row>
   </sheetData>

</xml_diff>